<commit_message>
update Korean New Deal reports
</commit_message>
<xml_diff>
--- a/data/한국판뉴딜.xlsx
+++ b/data/한국판뉴딜.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="90" windowWidth="26980" windowHeight="10200" activeTab="1"/>
+    <workbookView xWindow="320" yWindow="90" windowWidth="26980" windowHeight="10200" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="finance" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="EDA" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="51">
   <si>
     <t>레벨0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -191,6 +192,22 @@
   </si>
   <si>
     <t>일자리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 구축ㆍ개방ㆍ활용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공공시설 제로에너지화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초중고에 디지털 기반 교육 인프라 조성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대학ㆍ직업훈련기관 온라인 교육 강화</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1058,7 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1736,14 +1753,681 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2">
+        <v>6.4</v>
+      </c>
+      <c r="F2">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:C18" si="0">A2</f>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>디지털뉴딜</v>
+      </c>
+      <c r="C3" t="str">
+        <f>C2</f>
+        <v>D.N.A. 생태계 강화</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>14.8</v>
+      </c>
+      <c r="F3">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>디지털뉴딜</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>D.N.A. 생태계 강화</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F4">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>디지털뉴딜</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>D.N.A. 생태계 강화</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>디지털뉴딜</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6">
+        <v>0.3</v>
+      </c>
+      <c r="F6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>디지털뉴딜</v>
+      </c>
+      <c r="C7" t="str">
+        <f>C6</f>
+        <v>교육 인프라 디지털 전환</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>디지털뉴딜</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>0.4</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>디지털뉴딜</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>비대면 산업 육성</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>0.7</v>
+      </c>
+      <c r="F9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>디지털뉴딜</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>비대면 산업 육성</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>디지털뉴딜</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>8.5</v>
+      </c>
+      <c r="F11">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>디지털뉴딜</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>SOC 디지털화</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12">
+        <v>1.2</v>
+      </c>
+      <c r="F12">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>디지털뉴딜</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>SOC 디지털화</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>0.3</v>
+      </c>
+      <c r="F13">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14">
+        <v>6.2</v>
+      </c>
+      <c r="F14">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>그린뉴딜</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>도시ㆍ공간ㆍ생활 인프라 녹색 전환</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15">
+        <v>2.5</v>
+      </c>
+      <c r="F15">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>그린뉴딜</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>도시ㆍ공간ㆍ생활 인프라 녹색 전환</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16">
+        <v>3.4</v>
+      </c>
+      <c r="F16">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>그린뉴딜</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>그린뉴딜</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>저탄소‧분산형 에너지 확산</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F18">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" t="str">
+        <f t="shared" ref="A19:C29" si="1">A18</f>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="1"/>
+        <v>그린뉴딜</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>저탄소‧분산형 에너지 확산</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19">
+        <v>13.1</v>
+      </c>
+      <c r="F19">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" t="str">
+        <f t="shared" si="1"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="1"/>
+        <v>그린뉴딜</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <v>3.6</v>
+      </c>
+      <c r="F20">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" t="str">
+        <f t="shared" si="1"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="1"/>
+        <v>그린뉴딜</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>녹색산업혁신 생태계구축</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21">
+        <v>2.7</v>
+      </c>
+      <c r="F21">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" t="str">
+        <f t="shared" si="1"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22">
+        <v>3.2</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" t="str">
+        <f t="shared" si="1"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="1"/>
+        <v>안전망강화</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>고용ㆍ사회안전망</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23">
+        <v>10.4</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" t="str">
+        <f t="shared" si="1"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="1"/>
+        <v>안전망강화</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>고용ㆍ사회안전망</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24">
+        <v>7.2</v>
+      </c>
+      <c r="F24">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" t="str">
+        <f t="shared" si="1"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="1"/>
+        <v>안전망강화</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>고용ㆍ사회안전망</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25">
+        <v>1.2</v>
+      </c>
+      <c r="F25">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" t="str">
+        <f t="shared" si="1"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="1"/>
+        <v>안전망강화</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>고용ㆍ사회안전망</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26">
+        <v>0.6</v>
+      </c>
+      <c r="F26">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" t="str">
+        <f t="shared" si="1"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="1"/>
+        <v>안전망강화</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F27">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" t="str">
+        <f t="shared" si="1"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="1"/>
+        <v>안전망강화</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="1"/>
+        <v>사람투자</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F28">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" t="str">
+        <f t="shared" si="1"/>
+        <v>한국판 뉴딜</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="1"/>
+        <v>안전망강화</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="1"/>
+        <v>사람투자</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29">
+        <v>0.6</v>
+      </c>
+      <c r="F29">
+        <v>2.9</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1758,4 +2442,17 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>